<commit_message>
Hydroethanolic extract Excel data.
</commit_message>
<xml_diff>
--- a/Data/Antimicrobial_EthOH.xlsx
+++ b/Data/Antimicrobial_EthOH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F4ss0\Documents\Ikiam21062022\Proyecto Guayusa\Antimicrobial_I_guayusa\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64338C3-EE61-4051-A2D7-AF203FEFFD90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2DBBCE-6393-4EAC-B307-458A99903D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{AE241DF6-4FFC-4DF2-B60A-123CF49BB9C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="5" xr2:uid="{AE241DF6-4FFC-4DF2-B60A-123CF49BB9C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Escalas" sheetId="1" r:id="rId1"/>
@@ -105,8 +105,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -137,9 +138,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1037,9 +1039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EDF4562-F84F-4E28-9C36-EB3AC9F3CE7D}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:I27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1195,7 +1195,7 @@
         <f>AVERAGE(B4:B6)</f>
         <v>18.988666666666667</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <f>AVERAGE(C4:C6)</f>
         <v>6.0442803254486064</v>
       </c>
@@ -1203,7 +1203,7 @@
         <f t="shared" ref="D7" si="1">AVERAGE(D4:D6)</f>
         <v>79.751333333333335</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <f>AVERAGE(E4:E6)</f>
         <v>31.157333333333337</v>
       </c>
@@ -1211,7 +1211,7 @@
         <f t="shared" ref="F7:G7" si="2">AVERAGE(F4:F6)</f>
         <v>31.228999999999999</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="3">
         <f t="shared" si="2"/>
         <v>9.9404994356335994</v>
       </c>
@@ -1219,7 +1219,7 @@
         <f t="shared" ref="H7" si="3">AVERAGE(H4:H6)</f>
         <v>29.48</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="3">
         <f t="shared" ref="I7" si="4">AVERAGE(I4:I6)</f>
         <v>9.3837754446981485</v>
       </c>
@@ -1232,7 +1232,7 @@
         <f>_xlfn.STDEV.S(B4:B6)</f>
         <v>0.62358987590670034</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <f>_xlfn.STDEV.S(C4:C6)</f>
         <v>0.19849482242522551</v>
       </c>
@@ -1240,7 +1240,7 @@
         <f t="shared" ref="D8" si="5">_xlfn.STDEV.S(D4:D6)</f>
         <v>0.85621044920820921</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2">
         <f>_xlfn.STDEV.S(E4:E6)</f>
         <v>2.98250873147646</v>
       </c>
@@ -1248,7 +1248,7 @@
         <f t="shared" ref="F8:I8" si="6">_xlfn.STDEV.S(F4:F6)</f>
         <v>2.1469399153213375</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="2">
         <f t="shared" si="6"/>
         <v>0.68339220008937207</v>
       </c>
@@ -1256,7 +1256,7 @@
         <f t="shared" si="6"/>
         <v>2.0259977788734118</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="2">
         <f t="shared" si="6"/>
         <v>0.6448951224018078</v>
       </c>
@@ -1634,7 +1634,7 @@
         <f>AVERAGE(B24:B26)</f>
         <v>18.222333333333335</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="3">
         <f>AVERAGE(C24:C26)</f>
         <v>5.8003488493364275</v>
       </c>
@@ -1642,7 +1642,7 @@
         <f t="shared" ref="D27" si="16">AVERAGE(D24:D26)</f>
         <v>79.979666666666674</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="3">
         <f>AVERAGE(E24:E26)</f>
         <v>25.458318593684186</v>
       </c>
@@ -1650,7 +1650,7 @@
         <f t="shared" ref="F27" si="17">AVERAGE(F24:F26)</f>
         <v>55.479666666666667</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="3">
         <f t="shared" ref="G27" si="18">AVERAGE(G24:G26)</f>
         <v>17.659726382181312</v>
       </c>
@@ -1658,7 +1658,7 @@
         <f t="shared" ref="H27" si="19">AVERAGE(H24:H26)</f>
         <v>55.890333333333331</v>
       </c>
-      <c r="I27" s="2">
+      <c r="I27" s="3">
         <f t="shared" ref="I27" si="20">AVERAGE(I24:I26)</f>
         <v>17.790445642107457</v>
       </c>
@@ -1671,7 +1671,7 @@
         <f>_xlfn.STDEV.S(B24:B26)</f>
         <v>1.3463808277502076</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="2">
         <f>_xlfn.STDEV.S(C24:C26)</f>
         <v>0.42856632804120659</v>
       </c>
@@ -1679,7 +1679,7 @@
         <f t="shared" ref="D28" si="21">_xlfn.STDEV.S(D24:D26)</f>
         <v>0.54096426252880592</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" s="2">
         <f>_xlfn.STDEV.S(E24:E26)</f>
         <v>0.17219427283504152</v>
       </c>
@@ -1687,7 +1687,7 @@
         <f t="shared" ref="F28:I28" si="22">_xlfn.STDEV.S(F24:F26)</f>
         <v>1.6526658262738212</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28" s="2">
         <f t="shared" si="22"/>
         <v>0.526059871061061</v>
       </c>
@@ -1695,7 +1695,7 @@
         <f t="shared" si="22"/>
         <v>1.3432089686021826</v>
       </c>
-      <c r="I28" s="1">
+      <c r="I28" s="2">
         <f t="shared" si="22"/>
         <v>0.42755669391680884</v>
       </c>
@@ -1855,7 +1855,7 @@
         <f>AVERAGE(B34:B36)</f>
         <v>23.447666666666663</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="3">
         <f>AVERAGE(C34:C36)</f>
         <v>7.4636241079421302</v>
       </c>
@@ -1863,7 +1863,7 @@
         <f t="shared" ref="D37" si="24">AVERAGE(D34:D36)</f>
         <v>41.145333333333333</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E37" s="3">
         <f>AVERAGE(E34:E36)</f>
         <v>13.096966370327459</v>
       </c>
@@ -1871,7 +1871,7 @@
         <f t="shared" ref="F37:I37" si="25">AVERAGE(F34:F36)</f>
         <v>26.715666666666664</v>
       </c>
-      <c r="G37" s="1">
+      <c r="G37" s="3">
         <f t="shared" si="25"/>
         <v>8.5038608159907572</v>
       </c>
@@ -1879,7 +1879,7 @@
         <f t="shared" si="25"/>
         <v>36.966333333333331</v>
       </c>
-      <c r="I37" s="1">
+      <c r="I37" s="3">
         <f t="shared" si="25"/>
         <v>11.766749355965402</v>
       </c>
@@ -1892,7 +1892,7 @@
         <f>_xlfn.STDEV.S(B34:B36)</f>
         <v>2.4170255135875869</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="2">
         <f>_xlfn.STDEV.S(C34:C36)</f>
         <v>0.76936311613338337</v>
       </c>
@@ -1900,7 +1900,7 @@
         <f t="shared" ref="D38" si="26">_xlfn.STDEV.S(D34:D36)</f>
         <v>3.4538791717912383</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" s="2">
         <f>_xlfn.STDEV.S(E34:E36)</f>
         <v>1.0994038860654345</v>
       </c>
@@ -1908,7 +1908,7 @@
         <f t="shared" ref="F38:I38" si="27">_xlfn.STDEV.S(F34:F36)</f>
         <v>1.2356797049937069</v>
       </c>
-      <c r="G38" s="1">
+      <c r="G38" s="2">
         <f t="shared" si="27"/>
         <v>0.39332906625616648</v>
       </c>
@@ -1916,7 +1916,7 @@
         <f t="shared" si="27"/>
         <v>2.5900087515939658</v>
       </c>
-      <c r="I38" s="1">
+      <c r="I38" s="2">
         <f t="shared" si="27"/>
         <v>0.82442539093489731</v>
       </c>
@@ -2138,7 +2138,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60593CFE-100E-485A-AB91-C94FDA48628B}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>